<commit_message>
Modify US inventory to remove misc emissions for all except NH3
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/USA/national_tier1_caps.xlsx
+++ b/input/emissions-inventories/USA/national_tier1_caps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="14040" tabRatio="706" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="14040" tabRatio="706" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="VOC" sheetId="8" r:id="rId9"/>
     <sheet name="NH3" sheetId="9" r:id="rId10"/>
     <sheet name="NH3-Org_and_Adj" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="90">
   <si>
     <r>
       <rPr>
@@ -355,6 +356,9 @@
   </si>
   <si>
     <t>Trend Difference</t>
+  </si>
+  <si>
+    <t>CEDS Changes: "MISCELLANEOUS" sector zeroed out for all species except NH3 (emissions other than ag-waste-burning is zero for other species)</t>
   </si>
 </sst>
 </file>
@@ -862,7 +866,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="271">
+  <cellStyleXfs count="279">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -962,6 +966,14 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1329,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="271">
+  <cellStyles count="279">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="86"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
@@ -1463,6 +1475,10 @@
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1554,6 +1570,10 @@
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2523,11 +2543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121886056"/>
-        <c:axId val="-2121882904"/>
+        <c:axId val="2079372456"/>
+        <c:axId val="2079375624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2121886056"/>
+        <c:axId val="2079372456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1970.0"/>
@@ -2538,12 +2558,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121882904"/>
+        <c:crossAx val="2079375624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2121882904"/>
+        <c:axId val="2079375624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2566,13 +2586,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121886056"/>
+        <c:crossAx val="2079372456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3086,11 +3107,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121844008"/>
-        <c:axId val="-2121840984"/>
+        <c:axId val="2090156104"/>
+        <c:axId val="2090765304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2121844008"/>
+        <c:axId val="2090156104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1990.0"/>
@@ -3101,12 +3122,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121840984"/>
+        <c:crossAx val="2090765304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2121840984"/>
+        <c:axId val="2090765304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3136,7 +3157,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121844008"/>
+        <c:crossAx val="2090156104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3573,9 +3594,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -3584,164 +3607,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="4" t="s">
-        <v>70</v>
+      <c r="A1" s="88" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="28">
-      <c r="A3" s="91" t="s">
+    <row r="4" spans="1:1" ht="28">
+      <c r="A4" s="91" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="4"/>
-    </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="88" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="88" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="82" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" s="82" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:1">
+      <c r="A10" s="4" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="28">
-      <c r="A10" s="82" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="28">
       <c r="A11" s="82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="28">
+      <c r="A12" s="82" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="82" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="82" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="82"/>
-    </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="82"/>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="88" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="88" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="88" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="28">
-      <c r="A19" s="82" t="s">
+    <row r="20" spans="1:1" ht="28">
+      <c r="A20" s="82" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="82" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="82" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="82" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="4"/>
-    </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="88" t="s">
-        <v>0</v>
-      </c>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="88" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="88" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="88" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="88" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="266">
-      <c r="A29" s="82" t="s">
+    <row r="30" spans="1:1" ht="266">
+      <c r="A30" s="82" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="88" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="88" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="28">
-      <c r="A33" s="82" t="s">
+    <row r="34" spans="1:1" ht="28">
+      <c r="A34" s="82" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="70">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:1" ht="70">
+      <c r="A35" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="28">
-      <c r="A35" s="82" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="28">
       <c r="A36" s="82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="28">
       <c r="A37" s="82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="28">
+      <c r="A38" s="82" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6062,11 +6090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8619,6 +8647,23 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
@@ -8733,10 +8778,10 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AD12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10076,93 +10121,35 @@
       <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="67">
-        <v>7909</v>
-      </c>
-      <c r="C18" s="67">
-        <v>5263</v>
-      </c>
-      <c r="D18" s="67">
-        <v>8344</v>
-      </c>
-      <c r="E18" s="67">
-        <v>7927</v>
-      </c>
-      <c r="F18" s="67">
-        <v>11122</v>
-      </c>
-      <c r="G18" s="67">
-        <v>8618</v>
-      </c>
-      <c r="H18" s="67">
-        <v>6934</v>
-      </c>
-      <c r="I18" s="67">
-        <v>7082</v>
-      </c>
-      <c r="J18" s="67">
-        <v>9656</v>
-      </c>
-      <c r="K18" s="67">
-        <v>7298</v>
-      </c>
-      <c r="L18" s="67">
-        <v>15016.3282</v>
-      </c>
-      <c r="M18" s="67">
-        <v>7316.2786199999982</v>
-      </c>
-      <c r="N18" s="67">
-        <v>7184.1086699999969</v>
-      </c>
-      <c r="O18" s="67">
-        <v>11410.093849999996</v>
-      </c>
-      <c r="P18" s="67">
-        <v>12964.397550999998</v>
-      </c>
-      <c r="Q18" s="67">
-        <v>8675.5646280000001</v>
-      </c>
-      <c r="R18" s="85">
-        <v>18493.421145654007</v>
-      </c>
-      <c r="S18" s="90">
-        <v>19414.8205777406</v>
-      </c>
-      <c r="T18" s="90">
-        <v>20336.220009827193</v>
-      </c>
-      <c r="U18" s="90">
-        <v>15106.150261548795</v>
-      </c>
-      <c r="V18" s="90">
-        <v>17111.202873365368</v>
-      </c>
-      <c r="W18" s="85">
-        <v>19116.25548518194</v>
-      </c>
-      <c r="X18" s="85">
-        <v>21121.308047615032</v>
-      </c>
-      <c r="Y18" s="90">
-        <v>21839.417403587748</v>
-      </c>
-      <c r="Z18" s="90">
-        <v>22557.526759560464</v>
-      </c>
-      <c r="AA18" s="90">
-        <v>23776.943965482562</v>
-      </c>
-      <c r="AB18" s="90">
-        <v>23776.943965482562</v>
-      </c>
-      <c r="AC18" s="90">
-        <v>23776.943965482562</v>
-      </c>
-      <c r="AD18" s="90">
-        <v>23776.943965482562</v>
-      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="85"/>
+      <c r="X18" s="85"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="90"/>
+      <c r="AC18" s="90"/>
+      <c r="AD18" s="90"/>
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="8"/>
@@ -10250,55 +10237,55 @@
       </c>
       <c r="R20" s="90">
         <f>SUM(R6:R18)</f>
-        <v>102032.84772508191</v>
+        <v>83539.426579427905</v>
       </c>
       <c r="S20" s="90">
         <f t="shared" ref="S20:AD20" si="0">SUM(S6:S18)</f>
-        <v>99592.697940093363</v>
+        <v>80177.877362352767</v>
       </c>
       <c r="T20" s="90">
         <f t="shared" si="0"/>
-        <v>97147.153499984997</v>
+        <v>76810.933490157811</v>
       </c>
       <c r="U20" s="90">
         <f t="shared" si="0"/>
-        <v>88545.889554080597</v>
+        <v>73439.739292531798</v>
       </c>
       <c r="V20" s="90">
         <f t="shared" si="0"/>
-        <v>85837.099152230687</v>
+        <v>68725.896278865315</v>
       </c>
       <c r="W20" s="85">
         <f t="shared" si="0"/>
-        <v>83128.308750380776</v>
+        <v>64012.053265198832</v>
       </c>
       <c r="X20" s="85">
         <f t="shared" si="0"/>
-        <v>79655.089134955168</v>
+        <v>58533.781087340132</v>
       </c>
       <c r="Y20" s="85">
         <f t="shared" si="0"/>
-        <v>72752.52470155964</v>
+        <v>50913.107297971888</v>
       </c>
       <c r="Z20" s="85">
         <f t="shared" si="0"/>
-        <v>73771.049471133068</v>
+        <v>51213.522711572601</v>
       </c>
       <c r="AA20" s="85">
         <f t="shared" si="0"/>
-        <v>73761.574060525279</v>
+        <v>49984.63009504271</v>
       </c>
       <c r="AB20" s="90">
         <f t="shared" si="0"/>
-        <v>71759.784460010138</v>
+        <v>47982.840494527576</v>
       </c>
       <c r="AC20" s="90">
         <f t="shared" si="0"/>
-        <v>69757.994859494996</v>
+        <v>45981.050894012442</v>
       </c>
       <c r="AD20" s="90">
         <f t="shared" si="0"/>
-        <v>67756.20525897987</v>
+        <v>43979.261293497308</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -10447,55 +10434,55 @@
       </c>
       <c r="R22" s="90">
         <f>R20 - R21</f>
-        <v>87981.330673523145</v>
+        <v>69487.909527869138</v>
       </c>
       <c r="S22" s="90">
         <f t="shared" ref="S22:AD22" si="1">S20 - S21</f>
-        <v>85541.180888534596</v>
+        <v>66126.360310794</v>
       </c>
       <c r="T22" s="90">
         <f t="shared" si="1"/>
-        <v>83095.63644842623</v>
+        <v>62759.416438599044</v>
       </c>
       <c r="U22" s="90">
         <f t="shared" si="1"/>
-        <v>80645.841682886821</v>
+        <v>65539.691421338022</v>
       </c>
       <c r="V22" s="90">
         <f t="shared" si="1"/>
-        <v>77937.051281036911</v>
+        <v>60825.848407671539</v>
       </c>
       <c r="W22" s="85">
         <f t="shared" si="1"/>
-        <v>75228.260879187001</v>
+        <v>56112.005394005057</v>
       </c>
       <c r="X22" s="85">
         <f t="shared" si="1"/>
-        <v>67454.971152365266</v>
+        <v>46333.663104750231</v>
       </c>
       <c r="Y22" s="85">
         <f t="shared" si="1"/>
-        <v>60552.406718969738</v>
+        <v>38712.989315381987</v>
       </c>
       <c r="Z22" s="85">
         <f t="shared" si="1"/>
-        <v>61570.931488543167</v>
+        <v>39013.404728982699</v>
       </c>
       <c r="AA22" s="85">
         <f t="shared" si="1"/>
-        <v>61060.148227985999</v>
+        <v>37283.20426250343</v>
       </c>
       <c r="AB22" s="90">
         <f t="shared" si="1"/>
-        <v>59058.358627470858</v>
+        <v>35281.414661988296</v>
       </c>
       <c r="AC22" s="90">
         <f t="shared" si="1"/>
-        <v>57056.569026955716</v>
+        <v>33279.625061473162</v>
       </c>
       <c r="AD22" s="90">
         <f t="shared" si="1"/>
-        <v>55054.779426440589</v>
+        <v>31277.835460958027</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -10520,55 +10507,55 @@
       <c r="Q23" s="67"/>
       <c r="R23" s="90">
         <f t="shared" ref="R23:AD23" si="2">R18 - R21</f>
-        <v>4441.9040940952364</v>
+        <v>-14051.517051558771</v>
       </c>
       <c r="S23" s="90">
         <f t="shared" si="2"/>
-        <v>5363.3035261818295</v>
+        <v>-14051.517051558771</v>
       </c>
       <c r="T23" s="90">
         <f t="shared" si="2"/>
-        <v>6284.7029582684227</v>
+        <v>-14051.517051558771</v>
       </c>
       <c r="U23" s="90">
         <f t="shared" si="2"/>
-        <v>7206.1023903550176</v>
+        <v>-7900.0478711937776</v>
       </c>
       <c r="V23" s="90">
         <f t="shared" si="2"/>
-        <v>9211.1550021715902</v>
+        <v>-7900.0478711937776</v>
       </c>
       <c r="W23" s="85">
         <f t="shared" si="2"/>
-        <v>11216.207613988163</v>
+        <v>-7900.0478711937776</v>
       </c>
       <c r="X23" s="85">
         <f t="shared" si="2"/>
-        <v>8921.1900650251318</v>
+        <v>-12200.1179825899</v>
       </c>
       <c r="Y23" s="85">
         <f t="shared" si="2"/>
-        <v>9639.2994209978478</v>
+        <v>-12200.1179825899</v>
       </c>
       <c r="Z23" s="85">
         <f t="shared" si="2"/>
-        <v>10357.408776970564</v>
+        <v>-12200.1179825899</v>
       </c>
       <c r="AA23" s="85">
         <f t="shared" si="2"/>
-        <v>11075.51813294328</v>
+        <v>-12701.425832539282</v>
       </c>
       <c r="AB23" s="90">
         <f t="shared" si="2"/>
-        <v>11075.51813294328</v>
+        <v>-12701.425832539282</v>
       </c>
       <c r="AC23" s="90">
         <f t="shared" si="2"/>
-        <v>11075.51813294328</v>
+        <v>-12701.425832539282</v>
       </c>
       <c r="AD23" s="90">
         <f t="shared" si="2"/>
-        <v>11075.51813294328</v>
+        <v>-12701.425832539282</v>
       </c>
     </row>
     <row r="24" spans="1:30" s="65" customFormat="1">
@@ -11003,55 +10990,55 @@
       </c>
       <c r="R29" s="67">
         <f>R18</f>
-        <v>18493.421145654007</v>
+        <v>0</v>
       </c>
       <c r="S29" s="67">
         <f t="shared" ref="S29:AA29" si="9">S18</f>
-        <v>19414.8205777406</v>
+        <v>0</v>
       </c>
       <c r="T29" s="67">
         <f t="shared" si="9"/>
-        <v>20336.220009827193</v>
+        <v>0</v>
       </c>
       <c r="U29" s="67">
         <f t="shared" si="9"/>
-        <v>15106.150261548795</v>
+        <v>0</v>
       </c>
       <c r="V29" s="67">
         <f t="shared" si="9"/>
-        <v>17111.202873365368</v>
+        <v>0</v>
       </c>
       <c r="W29" s="67">
         <f t="shared" si="9"/>
-        <v>19116.25548518194</v>
+        <v>0</v>
       </c>
       <c r="X29" s="67">
         <f t="shared" si="9"/>
-        <v>21121.308047615032</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="67">
         <f t="shared" si="9"/>
-        <v>21839.417403587748</v>
+        <v>0</v>
       </c>
       <c r="Z29" s="67">
         <f t="shared" si="9"/>
-        <v>22557.526759560464</v>
+        <v>0</v>
       </c>
       <c r="AA29" s="67">
         <f t="shared" si="9"/>
-        <v>23776.943965482562</v>
+        <v>0</v>
       </c>
       <c r="AB29" s="90">
         <f t="shared" ref="AB29:AD29" si="10">AB18</f>
-        <v>23776.943965482562</v>
+        <v>0</v>
       </c>
       <c r="AC29" s="90">
         <f t="shared" si="10"/>
-        <v>23776.943965482562</v>
+        <v>0</v>
       </c>
       <c r="AD29" s="90">
         <f t="shared" si="10"/>
-        <v>23776.943965482562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -11108,55 +11095,55 @@
       </c>
       <c r="R30" s="67">
         <f>SUM(R26:R29)</f>
-        <v>102032.84772508191</v>
+        <v>83539.426579427905</v>
       </c>
       <c r="S30" s="67">
         <f t="shared" ref="S30:AA30" si="11">SUM(S26:S29)</f>
-        <v>99592.697940093363</v>
+        <v>80177.877362352767</v>
       </c>
       <c r="T30" s="67">
         <f t="shared" si="11"/>
-        <v>97147.153499984997</v>
+        <v>76810.933490157811</v>
       </c>
       <c r="U30" s="67">
         <f t="shared" si="11"/>
-        <v>88545.889554080612</v>
+        <v>73439.739292531813</v>
       </c>
       <c r="V30" s="67">
         <f t="shared" si="11"/>
-        <v>85837.099152230687</v>
+        <v>68725.896278865315</v>
       </c>
       <c r="W30" s="67">
         <f t="shared" si="11"/>
-        <v>83128.308750380776</v>
+        <v>64012.053265198832</v>
       </c>
       <c r="X30" s="67">
         <f t="shared" si="11"/>
-        <v>79655.089134955168</v>
+        <v>58533.781087340132</v>
       </c>
       <c r="Y30" s="67">
         <f t="shared" si="11"/>
-        <v>72752.52470155964</v>
+        <v>50913.107297971888</v>
       </c>
       <c r="Z30" s="67">
         <f t="shared" si="11"/>
-        <v>73771.049471133068</v>
+        <v>51213.522711572608</v>
       </c>
       <c r="AA30" s="67">
         <f t="shared" si="11"/>
-        <v>73761.574060525279</v>
+        <v>49984.63009504271</v>
       </c>
       <c r="AB30" s="90">
         <f t="shared" ref="AB30:AD30" si="12">SUM(AB26:AB29)</f>
-        <v>71759.784460010153</v>
+        <v>47982.840494527583</v>
       </c>
       <c r="AC30" s="90">
         <f t="shared" si="12"/>
-        <v>69757.994859494996</v>
+        <v>45981.050894012442</v>
       </c>
       <c r="AD30" s="90">
         <f t="shared" si="12"/>
-        <v>67756.20525897987</v>
+        <v>43979.261293497315</v>
       </c>
     </row>
     <row r="31" spans="1:30">
@@ -11218,8 +11205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="P70" sqref="P70"/>
@@ -14654,10 +14641,10 @@
   <dimension ref="A1:AF30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="R12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Y35" sqref="Y35"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16046,93 +16033,35 @@
       <c r="A18" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="86">
-        <v>330</v>
-      </c>
-      <c r="C18" s="86">
-        <v>165</v>
-      </c>
-      <c r="D18" s="86">
-        <v>248</v>
-      </c>
-      <c r="E18" s="86">
-        <v>310</v>
-      </c>
-      <c r="F18" s="86">
-        <v>369</v>
-      </c>
-      <c r="G18" s="86">
-        <v>286</v>
-      </c>
-      <c r="H18" s="86">
-        <v>255</v>
-      </c>
-      <c r="I18" s="86">
-        <v>241</v>
-      </c>
-      <c r="J18" s="86">
-        <v>390</v>
-      </c>
-      <c r="K18" s="86">
-        <v>267</v>
-      </c>
-      <c r="L18" s="86">
-        <v>412.36083000000002</v>
-      </c>
-      <c r="M18" s="86">
-        <v>186.56205</v>
-      </c>
-      <c r="N18" s="86">
-        <v>179.48262</v>
-      </c>
-      <c r="O18" s="86">
-        <v>251.008478</v>
-      </c>
-      <c r="P18" s="86">
-        <v>276.02077600000001</v>
-      </c>
-      <c r="Q18" s="86">
-        <v>184.00074600000002</v>
-      </c>
-      <c r="R18" s="90">
-        <v>210.5218700388956</v>
-      </c>
-      <c r="S18" s="90">
-        <v>178.22100162229688</v>
-      </c>
-      <c r="T18" s="90">
-        <v>145.92013320569814</v>
-      </c>
-      <c r="U18" s="90">
-        <v>270.91317886864238</v>
-      </c>
-      <c r="V18" s="90">
-        <v>267.78411331565155</v>
-      </c>
-      <c r="W18" s="90">
-        <v>264.65504776266073</v>
-      </c>
-      <c r="X18" s="90">
-        <v>261.51536351830242</v>
-      </c>
-      <c r="Y18" s="90">
-        <v>278.02373981873632</v>
-      </c>
-      <c r="Z18" s="90">
-        <v>294.53211611917015</v>
-      </c>
-      <c r="AA18" s="90">
-        <v>399.47283451301178</v>
-      </c>
-      <c r="AB18" s="90">
-        <v>399.47283451301178</v>
-      </c>
-      <c r="AC18" s="90">
-        <v>399.47283451301178</v>
-      </c>
-      <c r="AD18" s="90">
-        <v>399.47283451301178</v>
-      </c>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="90"/>
+      <c r="AC18" s="90"/>
+      <c r="AD18" s="90"/>
     </row>
     <row r="19" spans="1:30">
       <c r="B19" s="86"/>
@@ -16218,55 +16147,55 @@
       </c>
       <c r="R20" s="86">
         <f>SUM(R6:R18)</f>
-        <v>21849.551396946481</v>
+        <v>21639.029526907587</v>
       </c>
       <c r="S20" s="90">
         <f t="shared" ref="S20:AD20" si="0">SUM(S6:S18)</f>
-        <v>20736.103779919998</v>
+        <v>20557.882778297702</v>
       </c>
       <c r="T20" s="90">
         <f t="shared" si="0"/>
-        <v>19814.116095494443</v>
+        <v>19668.195962288744</v>
       </c>
       <c r="U20" s="90">
         <f t="shared" si="0"/>
-        <v>18926.876972542093</v>
+        <v>18655.963793673451</v>
       </c>
       <c r="V20" s="86">
         <f t="shared" si="0"/>
-        <v>17888.248803784358</v>
+        <v>17620.464690468707</v>
       </c>
       <c r="W20" s="86">
         <f t="shared" si="0"/>
-        <v>16849.6206350266</v>
+        <v>16584.965587263938</v>
       </c>
       <c r="X20" s="86">
         <f t="shared" si="0"/>
-        <v>15748.880257523624</v>
+        <v>15487.364894005321</v>
       </c>
       <c r="Y20" s="86">
         <f t="shared" si="0"/>
-        <v>14700.362533504338</v>
+        <v>14422.338793685602</v>
       </c>
       <c r="Z20" s="86">
         <f t="shared" si="0"/>
-        <v>13835.094764620875</v>
+        <v>13540.562648501706</v>
       </c>
       <c r="AA20" s="86">
         <f t="shared" si="0"/>
-        <v>13514.830522803384</v>
+        <v>13115.357688290373</v>
       </c>
       <c r="AB20" s="86">
         <f t="shared" si="0"/>
-        <v>12719.927214717522</v>
+        <v>12320.45438020451</v>
       </c>
       <c r="AC20" s="86">
         <f t="shared" si="0"/>
-        <v>12201.540323825056</v>
+        <v>11802.067489312045</v>
       </c>
       <c r="AD20" s="86">
         <f t="shared" si="0"/>
-        <v>11608.651647932593</v>
+        <v>11209.178813419581</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -16415,55 +16344,55 @@
       </c>
       <c r="R22" s="86">
         <f>R20 - R21</f>
-        <v>21735.932132157483</v>
+        <v>21525.410262118588</v>
       </c>
       <c r="S22" s="90">
         <f t="shared" ref="S22:AD22" si="1">S20 - S21</f>
-        <v>20622.484515131</v>
+        <v>20444.263513508704</v>
       </c>
       <c r="T22" s="90">
         <f t="shared" si="1"/>
-        <v>19700.496830705444</v>
+        <v>19554.576697499746</v>
       </c>
       <c r="U22" s="90">
         <f t="shared" si="1"/>
-        <v>18833.068016704816</v>
+        <v>18562.154837836173</v>
       </c>
       <c r="V22" s="86">
         <f t="shared" si="1"/>
-        <v>17794.43984794708</v>
+        <v>17526.655734631429</v>
       </c>
       <c r="W22" s="86">
         <f t="shared" si="1"/>
-        <v>16755.811679189323</v>
+        <v>16491.15663142666</v>
       </c>
       <c r="X22" s="86">
         <f t="shared" si="1"/>
-        <v>15652.510175117124</v>
+        <v>15390.994811598821</v>
       </c>
       <c r="Y22" s="86">
         <f t="shared" si="1"/>
-        <v>14603.992451097838</v>
+        <v>14325.968711279102</v>
       </c>
       <c r="Z22" s="86">
         <f t="shared" si="1"/>
-        <v>13738.724682214375</v>
+        <v>13444.192566095206</v>
       </c>
       <c r="AA22" s="86">
         <f t="shared" si="1"/>
-        <v>13330.028098303477</v>
+        <v>12930.555263790466</v>
       </c>
       <c r="AB22" s="86">
         <f t="shared" si="1"/>
-        <v>12535.124790217615</v>
+        <v>12135.651955704603</v>
       </c>
       <c r="AC22" s="86">
         <f t="shared" si="1"/>
-        <v>12016.73789932515</v>
+        <v>11617.265064812138</v>
       </c>
       <c r="AD22" s="86">
         <f t="shared" si="1"/>
-        <v>11423.849223432686</v>
+        <v>11024.376388919674</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -16476,103 +16405,103 @@
       <c r="E23" s="86"/>
       <c r="F23" s="86">
         <f t="shared" ref="F23:AD23" si="2">F18 - F21</f>
-        <v>7.3145800000000349</v>
+        <v>-361.68541999999997</v>
       </c>
       <c r="G23" s="86">
         <f t="shared" si="2"/>
-        <v>39.0642</v>
+        <v>-246.9358</v>
       </c>
       <c r="H23" s="86">
         <f t="shared" si="2"/>
-        <v>21.255109999999974</v>
+        <v>-233.74489000000003</v>
       </c>
       <c r="I23" s="86">
         <f t="shared" si="2"/>
-        <v>7.2551099999999735</v>
+        <v>-233.74489000000003</v>
       </c>
       <c r="J23" s="86">
         <f t="shared" si="2"/>
-        <v>8.316190000000006</v>
+        <v>-381.68380999999999</v>
       </c>
       <c r="K23" s="86">
         <f t="shared" si="2"/>
-        <v>8.8065899999999715</v>
+        <v>-258.19341000000003</v>
       </c>
       <c r="L23" s="86">
         <f t="shared" si="2"/>
-        <v>7.3745600000000309</v>
+        <v>-404.98626999999999</v>
       </c>
       <c r="M23" s="86">
         <f t="shared" si="2"/>
-        <v>7.445069999999987</v>
+        <v>-179.11698000000001</v>
       </c>
       <c r="N23" s="86">
         <f t="shared" si="2"/>
-        <v>7.5237699999999847</v>
+        <v>-171.95885000000001</v>
       </c>
       <c r="O23" s="86">
         <f t="shared" si="2"/>
-        <v>14.861007000000001</v>
+        <v>-236.147471</v>
       </c>
       <c r="P23" s="86">
         <f t="shared" si="2"/>
-        <v>12.819589000000008</v>
+        <v>-263.201187</v>
       </c>
       <c r="Q23" s="86">
         <f t="shared" si="2"/>
-        <v>13.036779000000024</v>
+        <v>-170.963967</v>
       </c>
       <c r="R23" s="86">
         <f t="shared" si="2"/>
-        <v>96.902605249895601</v>
+        <v>-113.619264789</v>
       </c>
       <c r="S23" s="90">
         <f t="shared" si="2"/>
-        <v>64.601736833296883</v>
+        <v>-113.619264789</v>
       </c>
       <c r="T23" s="90">
         <f t="shared" si="2"/>
-        <v>32.300868416698137</v>
+        <v>-113.619264789</v>
       </c>
       <c r="U23" s="90">
         <f t="shared" si="2"/>
-        <v>177.10422303136599</v>
+        <v>-93.808955837276386</v>
       </c>
       <c r="V23" s="86">
         <f t="shared" si="2"/>
-        <v>173.97515747837517</v>
+        <v>-93.808955837276386</v>
       </c>
       <c r="W23" s="86">
         <f t="shared" si="2"/>
-        <v>170.84609192538434</v>
+        <v>-93.808955837276386</v>
       </c>
       <c r="X23" s="86">
         <f t="shared" si="2"/>
-        <v>165.14528111180243</v>
+        <v>-96.370082406500003</v>
       </c>
       <c r="Y23" s="86">
         <f t="shared" si="2"/>
-        <v>181.65365741223633</v>
+        <v>-96.370082406500003</v>
       </c>
       <c r="Z23" s="86">
         <f t="shared" si="2"/>
-        <v>198.16203371267017</v>
+        <v>-96.370082406500003</v>
       </c>
       <c r="AA23" s="86">
         <f t="shared" si="2"/>
-        <v>214.67041001310403</v>
+        <v>-184.80242449990774</v>
       </c>
       <c r="AB23" s="86">
         <f t="shared" si="2"/>
-        <v>214.67041001310403</v>
+        <v>-184.80242449990774</v>
       </c>
       <c r="AC23" s="86">
         <f t="shared" si="2"/>
-        <v>214.67041001310403</v>
+        <v>-184.80242449990774</v>
       </c>
       <c r="AD23" s="86">
         <f t="shared" si="2"/>
-        <v>214.67041001310403</v>
+        <v>-184.80242449990774</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -17006,119 +16935,119 @@
       </c>
       <c r="B29" s="86">
         <f>B18</f>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="C29" s="86">
         <f t="shared" ref="C29:AD29" si="6">C18</f>
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="D29" s="86">
         <f t="shared" si="6"/>
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="E29" s="86">
         <f t="shared" si="6"/>
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="F29" s="86">
         <f t="shared" si="6"/>
-        <v>369</v>
+        <v>0</v>
       </c>
       <c r="G29" s="86">
         <f t="shared" si="6"/>
-        <v>286</v>
+        <v>0</v>
       </c>
       <c r="H29" s="86">
         <f t="shared" si="6"/>
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="I29" s="86">
         <f t="shared" si="6"/>
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="J29" s="86">
         <f t="shared" si="6"/>
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="K29" s="86">
         <f t="shared" si="6"/>
-        <v>267</v>
+        <v>0</v>
       </c>
       <c r="L29" s="86">
         <f t="shared" si="6"/>
-        <v>412.36083000000002</v>
+        <v>0</v>
       </c>
       <c r="M29" s="86">
         <f t="shared" si="6"/>
-        <v>186.56205</v>
+        <v>0</v>
       </c>
       <c r="N29" s="86">
         <f t="shared" si="6"/>
-        <v>179.48262</v>
+        <v>0</v>
       </c>
       <c r="O29" s="86">
         <f t="shared" si="6"/>
-        <v>251.008478</v>
+        <v>0</v>
       </c>
       <c r="P29" s="86">
         <f t="shared" si="6"/>
-        <v>276.02077600000001</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="86">
         <f t="shared" si="6"/>
-        <v>184.00074600000002</v>
+        <v>0</v>
       </c>
       <c r="R29" s="86">
         <f t="shared" si="6"/>
-        <v>210.5218700388956</v>
+        <v>0</v>
       </c>
       <c r="S29" s="86">
         <f t="shared" si="6"/>
-        <v>178.22100162229688</v>
+        <v>0</v>
       </c>
       <c r="T29" s="86">
         <f t="shared" si="6"/>
-        <v>145.92013320569814</v>
+        <v>0</v>
       </c>
       <c r="U29" s="86">
         <f t="shared" si="6"/>
-        <v>270.91317886864238</v>
+        <v>0</v>
       </c>
       <c r="V29" s="86">
         <f t="shared" si="6"/>
-        <v>267.78411331565155</v>
+        <v>0</v>
       </c>
       <c r="W29" s="86">
         <f t="shared" si="6"/>
-        <v>264.65504776266073</v>
+        <v>0</v>
       </c>
       <c r="X29" s="86">
         <f t="shared" si="6"/>
-        <v>261.51536351830242</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="86">
         <f t="shared" si="6"/>
-        <v>278.02373981873632</v>
+        <v>0</v>
       </c>
       <c r="Z29" s="86">
         <f t="shared" si="6"/>
-        <v>294.53211611917015</v>
+        <v>0</v>
       </c>
       <c r="AA29" s="86">
         <f t="shared" si="6"/>
-        <v>399.47283451301178</v>
+        <v>0</v>
       </c>
       <c r="AB29" s="86">
         <f t="shared" si="6"/>
-        <v>399.47283451301178</v>
+        <v>0</v>
       </c>
       <c r="AC29" s="86">
         <f t="shared" si="6"/>
-        <v>399.47283451301178</v>
+        <v>0</v>
       </c>
       <c r="AD29" s="86">
         <f t="shared" si="6"/>
-        <v>399.47283451301178</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -17127,119 +17056,119 @@
       </c>
       <c r="B30" s="86">
         <f>SUM(B26:B29)</f>
-        <v>26882</v>
+        <v>26552</v>
       </c>
       <c r="C30" s="86">
         <f t="shared" ref="C30:AD30" si="7">SUM(C26:C29)</f>
-        <v>26378</v>
+        <v>26213</v>
       </c>
       <c r="D30" s="86">
         <f t="shared" si="7"/>
-        <v>27080</v>
+        <v>26832</v>
       </c>
       <c r="E30" s="86">
         <f t="shared" si="7"/>
-        <v>25757</v>
+        <v>25447</v>
       </c>
       <c r="F30" s="86">
         <f t="shared" si="7"/>
-        <v>25527</v>
+        <v>25158</v>
       </c>
       <c r="G30" s="86">
         <f t="shared" si="7"/>
-        <v>25180</v>
+        <v>24894</v>
       </c>
       <c r="H30" s="86">
         <f t="shared" si="7"/>
-        <v>25261</v>
+        <v>25006</v>
       </c>
       <c r="I30" s="86">
         <f t="shared" si="7"/>
-        <v>25356</v>
+        <v>25115</v>
       </c>
       <c r="J30" s="86">
         <f t="shared" si="7"/>
-        <v>25350</v>
+        <v>24960</v>
       </c>
       <c r="K30" s="86">
         <f t="shared" si="7"/>
-        <v>24955</v>
+        <v>24688</v>
       </c>
       <c r="L30" s="86">
         <f t="shared" si="7"/>
-        <v>24787.361250000005</v>
+        <v>24375.000420000004</v>
       </c>
       <c r="M30" s="86">
         <f t="shared" si="7"/>
-        <v>24704.956589999998</v>
+        <v>24518.394539999998</v>
       </c>
       <c r="N30" s="86">
         <f t="shared" si="7"/>
-        <v>24596.103929938832</v>
+        <v>24416.621309938833</v>
       </c>
       <c r="O30" s="86">
         <f t="shared" si="7"/>
-        <v>23341.431169877669</v>
+        <v>23090.422691877669</v>
       </c>
       <c r="P30" s="86">
         <f t="shared" si="7"/>
-        <v>23343.465554816506</v>
+        <v>23067.444778816505</v>
       </c>
       <c r="Q30" s="86">
         <f t="shared" si="7"/>
-        <v>22691.163589955344</v>
+        <v>22507.162843955342</v>
       </c>
       <c r="R30" s="86">
         <f t="shared" si="7"/>
-        <v>21849.551396946481</v>
+        <v>21639.029526907587</v>
       </c>
       <c r="S30" s="86">
         <f t="shared" si="7"/>
-        <v>20736.103779920002</v>
+        <v>20557.882778297706</v>
       </c>
       <c r="T30" s="86">
         <f t="shared" si="7"/>
-        <v>19814.116095494443</v>
+        <v>19668.195962288744</v>
       </c>
       <c r="U30" s="86">
         <f t="shared" si="7"/>
-        <v>18926.876972542093</v>
+        <v>18655.963793673451</v>
       </c>
       <c r="V30" s="86">
         <f t="shared" si="7"/>
-        <v>17888.248803784361</v>
+        <v>17620.464690468711</v>
       </c>
       <c r="W30" s="86">
         <f t="shared" si="7"/>
-        <v>16849.6206350266</v>
+        <v>16584.965587263938</v>
       </c>
       <c r="X30" s="86">
         <f t="shared" si="7"/>
-        <v>15748.880257523624</v>
+        <v>15487.364894005321</v>
       </c>
       <c r="Y30" s="86">
         <f t="shared" si="7"/>
-        <v>14700.362533504338</v>
+        <v>14422.338793685602</v>
       </c>
       <c r="Z30" s="86">
         <f t="shared" si="7"/>
-        <v>13835.094764620875</v>
+        <v>13540.562648501706</v>
       </c>
       <c r="AA30" s="86">
         <f t="shared" si="7"/>
-        <v>13514.830522803384</v>
+        <v>13115.357688290373</v>
       </c>
       <c r="AB30" s="86">
         <f t="shared" si="7"/>
-        <v>12719.927214717523</v>
+        <v>12320.454380204512</v>
       </c>
       <c r="AC30" s="86">
         <f t="shared" si="7"/>
-        <v>12201.540323825056</v>
+        <v>11802.067489312045</v>
       </c>
       <c r="AD30" s="86">
         <f t="shared" si="7"/>
-        <v>11608.651647932593</v>
+        <v>11209.178813419581</v>
       </c>
     </row>
   </sheetData>
@@ -21259,13 +21188,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD30"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22509,7 +22438,7 @@
         <v>22.159243891632038</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:34">
       <c r="A17" s="40" t="s">
         <v>32</v>
       </c>
@@ -22601,99 +22530,45 @@
         <v>77.418929457120043</v>
       </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:34">
       <c r="A18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="44">
-        <v>110</v>
-      </c>
-      <c r="C18" s="44">
-        <v>20</v>
-      </c>
-      <c r="D18" s="44">
-        <v>11</v>
-      </c>
-      <c r="E18" s="44">
-        <v>11</v>
-      </c>
-      <c r="F18" s="44">
-        <v>12</v>
-      </c>
-      <c r="G18" s="44">
-        <v>11.85075</v>
-      </c>
-      <c r="H18" s="44">
-        <v>10</v>
-      </c>
-      <c r="I18" s="44">
-        <v>10</v>
-      </c>
-      <c r="J18" s="44">
-        <v>15</v>
-      </c>
-      <c r="K18" s="44">
-        <v>10</v>
-      </c>
-      <c r="L18" s="44">
-        <v>15.20858</v>
-      </c>
-      <c r="M18" s="44">
-        <v>6.6106699999999998</v>
-      </c>
-      <c r="N18" s="44">
-        <v>6.1332200000000006</v>
-      </c>
-      <c r="O18" s="44">
-        <v>67.435986999999997</v>
-      </c>
-      <c r="P18" s="44">
-        <v>69.539186999999998</v>
-      </c>
-      <c r="Q18" s="44">
-        <v>44.252963000000001</v>
-      </c>
-      <c r="R18" s="85">
-        <v>134.94766473039971</v>
-      </c>
-      <c r="S18" s="90">
-        <v>140.03166509695822</v>
-      </c>
-      <c r="T18" s="90">
-        <v>145.11566546351673</v>
-      </c>
-      <c r="U18" s="90">
-        <v>125.78046339385837</v>
-      </c>
-      <c r="V18" s="85">
-        <v>130.18024182856891</v>
-      </c>
-      <c r="W18" s="85">
-        <v>134.58002026327947</v>
-      </c>
-      <c r="X18" s="85">
-        <v>138.97816342146493</v>
-      </c>
-      <c r="Y18" s="90">
-        <v>149.88929388244762</v>
-      </c>
-      <c r="Z18" s="90">
-        <v>160.80042434343031</v>
-      </c>
-      <c r="AA18" s="90">
-        <v>197.55506837643335</v>
-      </c>
-      <c r="AB18" s="90">
-        <v>197.55506837643335</v>
-      </c>
-      <c r="AC18" s="90">
-        <v>197.55506837643335</v>
-      </c>
-      <c r="AD18" s="90">
-        <v>197.55506837643335</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30">
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="90"/>
+      <c r="AC18" s="90"/>
+      <c r="AD18" s="90"/>
+      <c r="AE18" s="88"/>
+      <c r="AF18" s="88"/>
+      <c r="AG18" s="88"/>
+      <c r="AH18" s="88"/>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19" s="37"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -22725,128 +22600,128 @@
       <c r="AC19" s="37"/>
       <c r="AD19" s="37"/>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:34">
       <c r="A20" s="45" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="44">
         <f>SUM(B6:B18)</f>
-        <v>31218</v>
+        <v>31108</v>
       </c>
       <c r="C20" s="73">
         <f t="shared" ref="C20:AA20" si="0">SUM(C6:C18)</f>
-        <v>28044</v>
+        <v>28024</v>
       </c>
       <c r="D20" s="73">
         <f t="shared" si="0"/>
-        <v>25926</v>
+        <v>25915</v>
       </c>
       <c r="E20" s="73">
         <f t="shared" si="0"/>
-        <v>23307</v>
+        <v>23296</v>
       </c>
       <c r="F20" s="73">
         <f t="shared" si="0"/>
-        <v>23077</v>
+        <v>23065</v>
       </c>
       <c r="G20" s="73">
         <f t="shared" si="0"/>
-        <v>22374.850750000001</v>
+        <v>22363</v>
       </c>
       <c r="H20" s="73">
         <f t="shared" si="0"/>
-        <v>22082</v>
+        <v>22072</v>
       </c>
       <c r="I20" s="73">
         <f t="shared" si="0"/>
-        <v>21773</v>
+        <v>21763</v>
       </c>
       <c r="J20" s="73">
         <f t="shared" si="0"/>
-        <v>21346</v>
+        <v>21331</v>
       </c>
       <c r="K20" s="73">
         <f t="shared" si="0"/>
-        <v>18619</v>
+        <v>18609</v>
       </c>
       <c r="L20" s="73">
         <f t="shared" si="0"/>
-        <v>18385.268459999996</v>
+        <v>18370.059879999997</v>
       </c>
       <c r="M20" s="73">
         <f t="shared" si="0"/>
-        <v>18839.865219999996</v>
+        <v>18833.254549999998</v>
       </c>
       <c r="N20" s="73">
         <f t="shared" si="0"/>
-        <v>18944.408070000001</v>
+        <v>18938.274850000002</v>
       </c>
       <c r="O20" s="73">
         <f t="shared" si="0"/>
-        <v>17545.485519000002</v>
+        <v>17478.049532000001</v>
       </c>
       <c r="P20" s="73">
         <f t="shared" si="0"/>
-        <v>16346.998164999997</v>
+        <v>16277.458977999997</v>
       </c>
       <c r="Q20" s="73">
         <f t="shared" si="0"/>
-        <v>15931.655637999998</v>
+        <v>15887.402674999998</v>
       </c>
       <c r="R20" s="90">
         <f t="shared" si="0"/>
-        <v>15032.064971951257</v>
+        <v>14897.117307220857</v>
       </c>
       <c r="S20" s="90">
         <f t="shared" si="0"/>
-        <v>14807.944022964759</v>
+        <v>14667.912357867801</v>
       </c>
       <c r="T20" s="90">
         <f t="shared" si="0"/>
-        <v>14571.443002309114</v>
+        <v>14426.327336845598</v>
       </c>
       <c r="U20" s="90">
         <f t="shared" si="0"/>
-        <v>14545.748475852128</v>
+        <v>14419.96801245827</v>
       </c>
       <c r="V20" s="73">
         <f t="shared" si="0"/>
-        <v>13122.556026637047</v>
+        <v>12992.375784808477</v>
       </c>
       <c r="W20" s="73">
         <f t="shared" si="0"/>
-        <v>11699.363577421958</v>
+        <v>11564.783557158678</v>
       </c>
       <c r="X20" s="73">
         <f t="shared" si="0"/>
-        <v>10323.657863075903</v>
+        <v>10184.679699654438</v>
       </c>
       <c r="Y20" s="73">
         <f t="shared" si="0"/>
-        <v>9089.2376586734899</v>
+        <v>8939.3483647910416</v>
       </c>
       <c r="Z20" s="73">
         <f t="shared" si="0"/>
-        <v>7732.2084151080562</v>
+        <v>7571.4079907646255</v>
       </c>
       <c r="AA20" s="73">
         <f t="shared" si="0"/>
-        <v>6478.8391670777019</v>
+        <v>6281.2840987012687</v>
       </c>
       <c r="AB20" s="87">
         <f t="shared" ref="AB20:AD20" si="1">SUM(AB6:AB18)</f>
-        <v>5193.0683950167468</v>
+        <v>4995.5133266403136</v>
       </c>
       <c r="AC20" s="87">
         <f t="shared" si="1"/>
-        <v>5098.3217049874265</v>
+        <v>4900.7666366109934</v>
       </c>
       <c r="AD20" s="87">
         <f t="shared" si="1"/>
-        <v>4991.2006689581058</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30">
+        <v>4793.6456005816726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21" s="72" t="s">
         <v>44</v>
       </c>
@@ -22938,249 +22813,249 @@
         <v>95.836581044620246</v>
       </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:34">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="77">
         <f>B20</f>
-        <v>31218</v>
+        <v>31108</v>
       </c>
       <c r="C22" s="77">
         <f t="shared" ref="C22:E22" si="2">C20</f>
-        <v>28044</v>
+        <v>28024</v>
       </c>
       <c r="D22" s="77">
         <f t="shared" si="2"/>
-        <v>25926</v>
+        <v>25915</v>
       </c>
       <c r="E22" s="77">
         <f t="shared" si="2"/>
-        <v>23307</v>
+        <v>23296</v>
       </c>
       <c r="F22" s="77">
         <f>F20 - F21</f>
-        <v>23065.149249999999</v>
+        <v>23053.149249999999</v>
       </c>
       <c r="G22" s="77">
         <f t="shared" ref="G22:AA22" si="3">G20 - G21</f>
-        <v>22363</v>
+        <v>22351.149249999999</v>
       </c>
       <c r="H22" s="77">
         <f t="shared" si="3"/>
-        <v>22072.74093</v>
+        <v>22062.74093</v>
       </c>
       <c r="I22" s="77">
         <f t="shared" si="3"/>
-        <v>21764.272980000002</v>
+        <v>21754.272980000002</v>
       </c>
       <c r="J22" s="77">
         <f t="shared" si="3"/>
-        <v>21331.508870000001</v>
+        <v>21316.508870000001</v>
       </c>
       <c r="K22" s="77">
         <f t="shared" si="3"/>
-        <v>18609.347389999999</v>
+        <v>18599.347389999999</v>
       </c>
       <c r="L22" s="77">
         <f t="shared" si="3"/>
-        <v>18370.474499999997</v>
+        <v>18355.265919999998</v>
       </c>
       <c r="M22" s="77">
         <f t="shared" si="3"/>
-        <v>18833.679719999996</v>
+        <v>18827.069049999998</v>
       </c>
       <c r="N22" s="77">
         <f t="shared" si="3"/>
-        <v>18938.707270000003</v>
+        <v>18932.574050000003</v>
       </c>
       <c r="O22" s="77">
         <f t="shared" si="3"/>
-        <v>17478.266265000002</v>
+        <v>17410.830278000001</v>
       </c>
       <c r="P22" s="77">
         <f t="shared" si="3"/>
-        <v>16277.676304999997</v>
+        <v>16208.137117999997</v>
       </c>
       <c r="Q22" s="77">
         <f t="shared" si="3"/>
-        <v>15887.624507999999</v>
+        <v>15843.371544999998</v>
       </c>
       <c r="R22" s="90">
         <f t="shared" si="3"/>
-        <v>14951.729595059256</v>
+        <v>14816.781930328856</v>
       </c>
       <c r="S22" s="90">
         <f t="shared" si="3"/>
-        <v>14727.608646072758</v>
+        <v>14587.5769809758</v>
       </c>
       <c r="T22" s="90">
         <f t="shared" si="3"/>
-        <v>14491.107625417113</v>
+        <v>14345.991959953597</v>
       </c>
       <c r="U22" s="90">
         <f t="shared" si="3"/>
-        <v>14489.832301396345</v>
+        <v>14364.051838002488</v>
       </c>
       <c r="V22" s="77">
         <f t="shared" si="3"/>
-        <v>13066.639852181264</v>
+        <v>12936.459610352695</v>
       </c>
       <c r="W22" s="77">
         <f t="shared" si="3"/>
-        <v>11643.447402966176</v>
+        <v>11508.867382702896</v>
       </c>
       <c r="X22" s="77">
         <f t="shared" si="3"/>
-        <v>10253.664795603303</v>
+        <v>10114.686632181838</v>
       </c>
       <c r="Y22" s="77">
         <f t="shared" si="3"/>
-        <v>9019.2445912008898</v>
+        <v>8869.3552973184414</v>
       </c>
       <c r="Z22" s="77">
         <f t="shared" si="3"/>
-        <v>7662.2153476354561</v>
+        <v>7501.4149232920254</v>
       </c>
       <c r="AA22" s="77">
         <f t="shared" si="3"/>
-        <v>6383.0025860330816</v>
+        <v>6185.4475176566484</v>
       </c>
       <c r="AB22" s="87">
         <f t="shared" ref="AB22:AD22" si="4">AB20 - AB21</f>
-        <v>5097.2318139721265</v>
+        <v>4899.6767455956933</v>
       </c>
       <c r="AC22" s="87">
         <f t="shared" si="4"/>
-        <v>5002.4851239428062</v>
+        <v>4804.9300555663731</v>
       </c>
       <c r="AD22" s="87">
         <f t="shared" si="4"/>
-        <v>4895.3640879134855</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
+        <v>4697.8090195370523</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" s="56" t="s">
         <v>45</v>
       </c>
       <c r="B23" s="77">
         <f>B18</f>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C23" s="77">
         <f t="shared" ref="C23:E23" si="5">C18</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D23" s="77">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E23" s="77">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F23" s="77">
         <f t="shared" ref="F23:AA23" si="6">F18 - F21</f>
-        <v>0.14925000000000033</v>
+        <v>-11.85075</v>
       </c>
       <c r="G23" s="77">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-11.85075</v>
       </c>
       <c r="H23" s="77">
         <f t="shared" si="6"/>
-        <v>0.74093000000000053</v>
+        <v>-9.2590699999999995</v>
       </c>
       <c r="I23" s="77">
         <f t="shared" si="6"/>
-        <v>1.2729800000000004</v>
+        <v>-8.7270199999999996</v>
       </c>
       <c r="J23" s="77">
         <f t="shared" si="6"/>
-        <v>0.50886999999999993</v>
+        <v>-14.49113</v>
       </c>
       <c r="K23" s="77">
         <f t="shared" si="6"/>
-        <v>0.34738999999999898</v>
+        <v>-9.652610000000001</v>
       </c>
       <c r="L23" s="77">
         <f t="shared" si="6"/>
-        <v>0.4146200000000011</v>
+        <v>-14.793959999999998</v>
       </c>
       <c r="M23" s="77">
         <f t="shared" si="6"/>
-        <v>0.4251699999999996</v>
+        <v>-6.1855000000000002</v>
       </c>
       <c r="N23" s="77">
         <f t="shared" si="6"/>
-        <v>0.43242000000000047</v>
+        <v>-5.7008000000000001</v>
       </c>
       <c r="O23" s="77">
         <f t="shared" si="6"/>
-        <v>0.21673299999999074</v>
+        <v>-67.219254000000006</v>
       </c>
       <c r="P23" s="77">
         <f t="shared" si="6"/>
-        <v>0.21732699999999738</v>
+        <v>-69.321860000000001</v>
       </c>
       <c r="Q23" s="77">
         <f t="shared" si="6"/>
-        <v>0.22183300000000372</v>
+        <v>-44.031129999999997</v>
       </c>
       <c r="R23" s="90">
         <f t="shared" si="6"/>
-        <v>54.612287838399936</v>
+        <v>-80.335376891999772</v>
       </c>
       <c r="S23" s="90">
         <f t="shared" si="6"/>
-        <v>59.696288204958449</v>
+        <v>-80.335376891999772</v>
       </c>
       <c r="T23" s="90">
         <f t="shared" si="6"/>
-        <v>64.780288571516962</v>
+        <v>-80.335376891999772</v>
       </c>
       <c r="U23" s="90">
         <f t="shared" si="6"/>
-        <v>69.864288938075475</v>
+        <v>-55.916174455782894</v>
       </c>
       <c r="V23" s="77">
         <f t="shared" si="6"/>
-        <v>74.264067372786016</v>
+        <v>-55.916174455782894</v>
       </c>
       <c r="W23" s="77">
         <f t="shared" si="6"/>
-        <v>78.663845807496571</v>
+        <v>-55.916174455782894</v>
       </c>
       <c r="X23" s="77">
         <f t="shared" si="6"/>
-        <v>68.985095948865023</v>
+        <v>-69.993067472599904</v>
       </c>
       <c r="Y23" s="77">
         <f t="shared" si="6"/>
-        <v>79.896226409847714</v>
+        <v>-69.993067472599904</v>
       </c>
       <c r="Z23" s="77">
         <f t="shared" si="6"/>
-        <v>90.807356870830404</v>
+        <v>-69.993067472599904</v>
       </c>
       <c r="AA23" s="77">
         <f t="shared" si="6"/>
-        <v>101.71848733181311</v>
+        <v>-95.836581044620246</v>
       </c>
       <c r="AB23" s="87">
         <f t="shared" ref="AB23:AD23" si="7">AB18 - AB21</f>
-        <v>101.71848733181311</v>
+        <v>-95.836581044620246</v>
       </c>
       <c r="AC23" s="87">
         <f t="shared" si="7"/>
-        <v>101.71848733181311</v>
+        <v>-95.836581044620246</v>
       </c>
       <c r="AD23" s="87">
         <f t="shared" si="7"/>
-        <v>101.71848733181311</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30">
+        <v>-95.836581044620246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24" s="38"/>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -23212,7 +23087,7 @@
       <c r="AC24" s="37"/>
       <c r="AD24" s="37"/>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:34">
       <c r="A25" s="38"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -23244,7 +23119,7 @@
       <c r="AC25" s="37"/>
       <c r="AD25" s="37"/>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:34">
       <c r="A26" s="56" t="s">
         <v>46</v>
       </c>
@@ -23365,7 +23240,7 @@
         <v>4089.2870083871212</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:34">
       <c r="A27" s="56" t="s">
         <v>47</v>
       </c>
@@ -23486,7 +23361,7 @@
         <v>604.7804188458</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:34">
       <c r="A28" s="56" t="s">
         <v>48</v>
       </c>
@@ -23607,246 +23482,246 @@
         <v>99.578173348752074</v>
       </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:34">
       <c r="A29" s="56" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="75">
         <f>B18</f>
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C29" s="75">
         <f t="shared" ref="C29:AA29" si="14">C18</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D29" s="75">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E29" s="75">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F29" s="75">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G29" s="75">
         <f t="shared" si="14"/>
-        <v>11.85075</v>
+        <v>0</v>
       </c>
       <c r="H29" s="75">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I29" s="75">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J29" s="75">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="K29" s="75">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L29" s="75">
         <f t="shared" si="14"/>
-        <v>15.20858</v>
+        <v>0</v>
       </c>
       <c r="M29" s="75">
         <f t="shared" si="14"/>
-        <v>6.6106699999999998</v>
+        <v>0</v>
       </c>
       <c r="N29" s="75">
         <f t="shared" si="14"/>
-        <v>6.1332200000000006</v>
+        <v>0</v>
       </c>
       <c r="O29" s="75">
         <f t="shared" si="14"/>
-        <v>67.435986999999997</v>
+        <v>0</v>
       </c>
       <c r="P29" s="75">
         <f t="shared" si="14"/>
-        <v>69.539186999999998</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="75">
         <f t="shared" si="14"/>
-        <v>44.252963000000001</v>
+        <v>0</v>
       </c>
       <c r="R29" s="75">
         <f t="shared" si="14"/>
-        <v>134.94766473039971</v>
+        <v>0</v>
       </c>
       <c r="S29" s="75">
         <f t="shared" si="14"/>
-        <v>140.03166509695822</v>
+        <v>0</v>
       </c>
       <c r="T29" s="75">
         <f t="shared" si="14"/>
-        <v>145.11566546351673</v>
+        <v>0</v>
       </c>
       <c r="U29" s="75">
         <f t="shared" si="14"/>
-        <v>125.78046339385837</v>
+        <v>0</v>
       </c>
       <c r="V29" s="75">
         <f t="shared" si="14"/>
-        <v>130.18024182856891</v>
+        <v>0</v>
       </c>
       <c r="W29" s="75">
         <f t="shared" si="14"/>
-        <v>134.58002026327947</v>
+        <v>0</v>
       </c>
       <c r="X29" s="75">
         <f t="shared" si="14"/>
-        <v>138.97816342146493</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="75">
         <f t="shared" si="14"/>
-        <v>149.88929388244762</v>
+        <v>0</v>
       </c>
       <c r="Z29" s="75">
         <f t="shared" si="14"/>
-        <v>160.80042434343031</v>
+        <v>0</v>
       </c>
       <c r="AA29" s="75">
         <f t="shared" si="14"/>
-        <v>197.55506837643335</v>
+        <v>0</v>
       </c>
       <c r="AB29" s="84">
         <f t="shared" ref="AB29:AD29" si="15">AB18</f>
-        <v>197.55506837643335</v>
+        <v>0</v>
       </c>
       <c r="AC29" s="84">
         <f t="shared" si="15"/>
-        <v>197.55506837643335</v>
+        <v>0</v>
       </c>
       <c r="AD29" s="84">
         <f t="shared" si="15"/>
-        <v>197.55506837643335</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30" s="56" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="75">
         <f>SUM(B26:B29)</f>
-        <v>31218</v>
+        <v>31108</v>
       </c>
       <c r="C30" s="75">
         <f t="shared" ref="C30:AA30" si="16">SUM(C26:C29)</f>
-        <v>28044</v>
+        <v>28024</v>
       </c>
       <c r="D30" s="75">
         <f t="shared" si="16"/>
-        <v>25926</v>
+        <v>25915</v>
       </c>
       <c r="E30" s="75">
         <f t="shared" si="16"/>
-        <v>23307</v>
+        <v>23296</v>
       </c>
       <c r="F30" s="75">
         <f t="shared" si="16"/>
-        <v>23077</v>
+        <v>23065</v>
       </c>
       <c r="G30" s="75">
         <f t="shared" si="16"/>
-        <v>22374.850750000001</v>
+        <v>22363</v>
       </c>
       <c r="H30" s="75">
         <f t="shared" si="16"/>
-        <v>22082</v>
+        <v>22072</v>
       </c>
       <c r="I30" s="75">
         <f t="shared" si="16"/>
-        <v>21773</v>
+        <v>21763</v>
       </c>
       <c r="J30" s="75">
         <f t="shared" si="16"/>
-        <v>21346</v>
+        <v>21331</v>
       </c>
       <c r="K30" s="75">
         <f t="shared" si="16"/>
-        <v>18619</v>
+        <v>18609</v>
       </c>
       <c r="L30" s="75">
         <f t="shared" si="16"/>
-        <v>18385.268459999999</v>
+        <v>18370.059880000001</v>
       </c>
       <c r="M30" s="75">
         <f t="shared" si="16"/>
-        <v>18839.865219999992</v>
+        <v>18833.254549999994</v>
       </c>
       <c r="N30" s="75">
         <f t="shared" si="16"/>
-        <v>18944.408070000001</v>
+        <v>18938.274850000002</v>
       </c>
       <c r="O30" s="75">
         <f t="shared" si="16"/>
-        <v>17545.485518999998</v>
+        <v>17478.049531999997</v>
       </c>
       <c r="P30" s="75">
         <f t="shared" si="16"/>
-        <v>16346.998164999999</v>
+        <v>16277.458977999999</v>
       </c>
       <c r="Q30" s="75">
         <f t="shared" si="16"/>
-        <v>15931.655638</v>
+        <v>15887.402674999999</v>
       </c>
       <c r="R30" s="75">
         <f t="shared" si="16"/>
-        <v>15032.064971951257</v>
+        <v>14897.117307220857</v>
       </c>
       <c r="S30" s="75">
         <f t="shared" si="16"/>
-        <v>14807.944022964755</v>
+        <v>14667.912357867797</v>
       </c>
       <c r="T30" s="75">
         <f t="shared" si="16"/>
-        <v>14571.443002309112</v>
+        <v>14426.327336845596</v>
       </c>
       <c r="U30" s="75">
         <f t="shared" si="16"/>
-        <v>14545.748475852128</v>
+        <v>14419.96801245827</v>
       </c>
       <c r="V30" s="75">
         <f t="shared" si="16"/>
-        <v>13122.556026637043</v>
+        <v>12992.375784808473</v>
       </c>
       <c r="W30" s="75">
         <f t="shared" si="16"/>
-        <v>11699.363577421958</v>
+        <v>11564.783557158678</v>
       </c>
       <c r="X30" s="75">
         <f t="shared" si="16"/>
-        <v>10323.6578630759</v>
+        <v>10184.679699654434</v>
       </c>
       <c r="Y30" s="75">
         <f t="shared" si="16"/>
-        <v>9089.2376586734881</v>
+        <v>8939.3483647910398</v>
       </c>
       <c r="Z30" s="75">
         <f t="shared" si="16"/>
-        <v>7732.2084151080553</v>
+        <v>7571.4079907646246</v>
       </c>
       <c r="AA30" s="75">
         <f t="shared" si="16"/>
-        <v>6478.8391670777037</v>
+        <v>6281.2840987012705</v>
       </c>
       <c r="AB30" s="84">
         <f t="shared" ref="AB30:AD30" si="17">SUM(AB26:AB29)</f>
-        <v>5193.0683950167468</v>
+        <v>4995.5133266403136</v>
       </c>
       <c r="AC30" s="84">
         <f t="shared" si="17"/>
-        <v>5098.3217049874274</v>
+        <v>4900.7666366109943</v>
       </c>
       <c r="AD30" s="84">
         <f t="shared" si="17"/>
-        <v>4991.2006689581067</v>
+        <v>4793.6456005816735</v>
       </c>
     </row>
   </sheetData>
@@ -23862,13 +23737,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AH29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17:AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -25172,99 +25047,45 @@
         <v>1845.2317590219968</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:34">
       <c r="A17" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="53">
-        <v>1101</v>
-      </c>
-      <c r="C17" s="53">
-        <v>716</v>
-      </c>
-      <c r="D17" s="53">
-        <v>1134</v>
-      </c>
-      <c r="E17" s="53">
-        <v>566</v>
-      </c>
-      <c r="F17" s="53">
-        <v>1059</v>
-      </c>
-      <c r="G17" s="53">
-        <v>756</v>
-      </c>
-      <c r="H17" s="53">
-        <v>486</v>
-      </c>
-      <c r="I17" s="53">
-        <v>556</v>
-      </c>
-      <c r="J17" s="53">
-        <v>720</v>
-      </c>
-      <c r="K17" s="53">
-        <v>551</v>
-      </c>
-      <c r="L17" s="53">
-        <v>1940.443</v>
-      </c>
-      <c r="M17" s="53">
-        <v>815.92899999999997</v>
-      </c>
-      <c r="N17" s="53">
-        <v>717.85</v>
-      </c>
-      <c r="O17" s="53">
-        <v>791.077</v>
-      </c>
-      <c r="P17" s="53">
-        <v>733.03200000000004</v>
-      </c>
-      <c r="Q17" s="53">
-        <v>532.48900000000003</v>
-      </c>
-      <c r="R17" s="85">
-        <v>3970.3082495268764</v>
-      </c>
-      <c r="S17" s="90">
-        <v>4192.6286449138051</v>
-      </c>
-      <c r="T17" s="90">
-        <v>4414.949040300733</v>
-      </c>
-      <c r="U17" s="90">
-        <v>3291.4639995021262</v>
-      </c>
-      <c r="V17" s="85">
-        <v>3759.4718080810035</v>
-      </c>
-      <c r="W17" s="85">
-        <v>4227.4796166598808</v>
-      </c>
-      <c r="X17" s="85">
-        <v>4695.487388726503</v>
-      </c>
-      <c r="Y17" s="90">
-        <v>4878.8951776095064</v>
-      </c>
-      <c r="Z17" s="90">
-        <v>5062.3029664925089</v>
-      </c>
-      <c r="AA17" s="90">
-        <v>5290.3481356922075</v>
-      </c>
-      <c r="AB17" s="90">
-        <v>5290.3481356922075</v>
-      </c>
-      <c r="AC17" s="90">
-        <v>5290.3481356922075</v>
-      </c>
-      <c r="AD17" s="90">
-        <v>5290.3481356922075</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30">
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="90"/>
+      <c r="P17" s="90"/>
+      <c r="Q17" s="90"/>
+      <c r="R17" s="90"/>
+      <c r="S17" s="90"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="90"/>
+      <c r="V17" s="90"/>
+      <c r="W17" s="90"/>
+      <c r="X17" s="90"/>
+      <c r="Y17" s="90"/>
+      <c r="Z17" s="90"/>
+      <c r="AA17" s="90"/>
+      <c r="AB17" s="90"/>
+      <c r="AC17" s="90"/>
+      <c r="AD17" s="90"/>
+      <c r="AE17" s="88"/>
+      <c r="AF17" s="88"/>
+      <c r="AG17" s="88"/>
+      <c r="AH17" s="88"/>
+    </row>
+    <row r="18" spans="1:34">
       <c r="A18" s="46"/>
       <c r="B18" s="53"/>
       <c r="C18" s="53"/>
@@ -25296,7 +25117,7 @@
       <c r="AC18" s="53"/>
       <c r="AD18" s="46"/>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:34">
       <c r="A19" s="54" t="s">
         <v>36</v>
       </c>
@@ -25350,58 +25171,58 @@
       </c>
       <c r="R19" s="90">
         <f>SUM(R5:R17)</f>
-        <v>20289.449086873432</v>
+        <v>16319.140837346557</v>
       </c>
       <c r="S19" s="90">
         <f t="shared" ref="S19:AA19" si="0">SUM(S5:S17)</f>
-        <v>19910.969988720197</v>
+        <v>15718.341343806393</v>
       </c>
       <c r="T19" s="90">
         <f t="shared" si="0"/>
-        <v>19513.838971111792</v>
+        <v>15098.889930811061</v>
       </c>
       <c r="U19" s="90">
         <f t="shared" si="0"/>
-        <v>17753.005659169496</v>
+        <v>14461.541659667368</v>
       </c>
       <c r="V19" s="87">
         <f t="shared" si="0"/>
-        <v>17901.738045132202</v>
+        <v>14142.266237051201</v>
       </c>
       <c r="W19" s="87">
         <f t="shared" si="0"/>
-        <v>18050.470431094916</v>
+        <v>13822.990814435034</v>
       </c>
       <c r="X19" s="87">
         <f t="shared" si="0"/>
-        <v>17758.856144507652</v>
+        <v>13063.36875578115</v>
       </c>
       <c r="Y19" s="87">
         <f t="shared" si="0"/>
-        <v>17593.197218669509</v>
+        <v>12714.302041060002</v>
       </c>
       <c r="Z19" s="87">
         <f t="shared" si="0"/>
-        <v>17835.013588387945</v>
+        <v>12772.710621895436</v>
       </c>
       <c r="AA19" s="87">
         <f t="shared" si="0"/>
-        <v>18154.286815938198</v>
+        <v>12863.938680245989</v>
       </c>
       <c r="AB19" s="87">
         <f t="shared" ref="AB19:AD19" si="1">SUM(AB5:AB17)</f>
-        <v>17812.738867690328</v>
+        <v>12522.390731998119</v>
       </c>
       <c r="AC19" s="87">
         <f t="shared" si="1"/>
-        <v>17471.190919442459</v>
+        <v>12180.842783750251</v>
       </c>
       <c r="AD19" s="87">
         <f t="shared" si="1"/>
-        <v>17129.642971194589</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
+        <v>11839.294835502382</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20" s="76" t="s">
         <v>44</v>
       </c>
@@ -25493,7 +25314,7 @@
         <v>2891.2714002396851</v>
       </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:34">
       <c r="A21" s="76" t="s">
         <v>50</v>
       </c>
@@ -25563,179 +25384,179 @@
       </c>
       <c r="R21" s="90">
         <f t="shared" si="2"/>
-        <v>17075.974109372448</v>
+        <v>13105.665859845572</v>
       </c>
       <c r="S21" s="90">
         <f t="shared" si="2"/>
-        <v>16697.495011219213</v>
+        <v>12504.86636630541</v>
       </c>
       <c r="T21" s="90">
         <f t="shared" si="2"/>
-        <v>16300.363993610808</v>
+        <v>11885.414953310079</v>
       </c>
       <c r="U21" s="90">
         <f t="shared" si="2"/>
-        <v>15885.336117854047</v>
+        <v>12593.872118351919</v>
       </c>
       <c r="V21" s="79">
         <f t="shared" si="2"/>
-        <v>16034.068503816754</v>
+        <v>12274.596695735752</v>
       </c>
       <c r="W21" s="79">
         <f t="shared" si="2"/>
-        <v>16182.800889779468</v>
+        <v>11955.321273119585</v>
       </c>
       <c r="X21" s="79">
         <f t="shared" si="2"/>
-        <v>14912.222124584663</v>
+        <v>10216.734735858161</v>
       </c>
       <c r="Y21" s="79">
         <f t="shared" si="2"/>
-        <v>14746.56319874652</v>
+        <v>9867.6680211370112</v>
       </c>
       <c r="Z21" s="79">
         <f t="shared" si="2"/>
-        <v>14988.379568464956</v>
+        <v>9926.076601972447</v>
       </c>
       <c r="AA21" s="79">
         <f t="shared" si="2"/>
-        <v>15263.015415698512</v>
+        <v>9972.6672800063025</v>
       </c>
       <c r="AB21" s="87">
         <f t="shared" ref="AB21:AD21" si="3">AB19 - AB20</f>
-        <v>14921.467467450642</v>
+        <v>9631.119331758433</v>
       </c>
       <c r="AC21" s="87">
         <f t="shared" si="3"/>
-        <v>14579.919519202773</v>
+        <v>9289.5713835105671</v>
       </c>
       <c r="AD21" s="87">
         <f t="shared" si="3"/>
-        <v>14238.371570954903</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30">
+        <v>8948.0234352626976</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="79">
         <f t="shared" ref="B22:AA22" si="4">B17 - B20</f>
-        <v>184</v>
+        <v>-917</v>
       </c>
       <c r="C22" s="79">
         <f t="shared" si="4"/>
-        <v>129</v>
+        <v>-587</v>
       </c>
       <c r="D22" s="79">
         <f t="shared" si="4"/>
-        <v>110</v>
+        <v>-1024</v>
       </c>
       <c r="E22" s="79">
         <f t="shared" si="4"/>
-        <v>101</v>
+        <v>-465</v>
       </c>
       <c r="F22" s="79">
         <f t="shared" si="4"/>
-        <v>76</v>
+        <v>-983</v>
       </c>
       <c r="G22" s="79">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>-678</v>
       </c>
       <c r="H22" s="79">
         <f t="shared" si="4"/>
-        <v>79</v>
+        <v>-407</v>
       </c>
       <c r="I22" s="79">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>-478</v>
       </c>
       <c r="J22" s="79">
         <f t="shared" si="4"/>
-        <v>82</v>
+        <v>-638</v>
       </c>
       <c r="K22" s="79">
         <f t="shared" si="4"/>
-        <v>87</v>
+        <v>-464</v>
       </c>
       <c r="L22" s="79">
         <f t="shared" si="4"/>
-        <v>70.548999999999978</v>
+        <v>-1869.894</v>
       </c>
       <c r="M22" s="79">
         <f t="shared" si="4"/>
-        <v>71.638229999999908</v>
+        <v>-744.29077000000007</v>
       </c>
       <c r="N22" s="79">
         <f t="shared" si="4"/>
-        <v>72.442270000000008</v>
+        <v>-645.40773000000002</v>
       </c>
       <c r="O22" s="79">
         <f t="shared" si="4"/>
-        <v>124.03757599999983</v>
+        <v>-667.03942400000017</v>
       </c>
       <c r="P22" s="79">
         <f t="shared" si="4"/>
-        <v>118.19843100000014</v>
+        <v>-614.8335689999999</v>
       </c>
       <c r="Q22" s="79">
         <f t="shared" si="4"/>
-        <v>120.16065099999992</v>
+        <v>-412.32834900000012</v>
       </c>
       <c r="R22" s="90">
         <f t="shared" si="4"/>
-        <v>756.83327202589317</v>
+        <v>-3213.4749775009832</v>
       </c>
       <c r="S22" s="90">
         <f t="shared" si="4"/>
-        <v>979.15366741282196</v>
+        <v>-3213.4749775009832</v>
       </c>
       <c r="T22" s="90">
         <f t="shared" si="4"/>
-        <v>1201.4740627997498</v>
+        <v>-3213.4749775009832</v>
       </c>
       <c r="U22" s="90">
         <f t="shared" si="4"/>
-        <v>1423.794458186678</v>
+        <v>-1867.6695413154482</v>
       </c>
       <c r="V22" s="79">
         <f t="shared" si="4"/>
-        <v>1891.8022667655553</v>
+        <v>-1867.6695413154482</v>
       </c>
       <c r="W22" s="79">
         <f t="shared" si="4"/>
-        <v>2359.8100753444323</v>
+        <v>-1867.6695413154482</v>
       </c>
       <c r="X22" s="79">
         <f t="shared" si="4"/>
-        <v>1848.8533688035131</v>
+        <v>-2846.6340199229899</v>
       </c>
       <c r="Y22" s="79">
         <f t="shared" si="4"/>
-        <v>2032.2611576865165</v>
+        <v>-2846.6340199229899</v>
       </c>
       <c r="Z22" s="79">
         <f t="shared" si="4"/>
-        <v>2215.668946569519</v>
+        <v>-2846.6340199229899</v>
       </c>
       <c r="AA22" s="79">
         <f t="shared" si="4"/>
-        <v>2399.0767354525224</v>
+        <v>-2891.2714002396851</v>
       </c>
       <c r="AB22" s="87">
         <f t="shared" ref="AB22:AD22" si="5">AB17 - AB20</f>
-        <v>2399.0767354525224</v>
+        <v>-2891.2714002396851</v>
       </c>
       <c r="AC22" s="87">
         <f t="shared" si="5"/>
-        <v>2399.0767354525224</v>
+        <v>-2891.2714002396851</v>
       </c>
       <c r="AD22" s="87">
         <f t="shared" si="5"/>
-        <v>2399.0767354525224</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30">
+        <v>-2891.2714002396851</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23" s="47"/>
       <c r="B23" s="79"/>
       <c r="C23" s="79"/>
@@ -25767,7 +25588,7 @@
       <c r="AC23" s="79"/>
       <c r="AD23" s="46"/>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:34">
       <c r="A24" s="47"/>
       <c r="B24" s="79"/>
       <c r="C24" s="79"/>
@@ -25799,7 +25620,7 @@
       <c r="AC24" s="79"/>
       <c r="AD24" s="46"/>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:34">
       <c r="A25" s="56" t="s">
         <v>46</v>
       </c>
@@ -25920,7 +25741,7 @@
         <v>628.49656739682018</v>
       </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:34">
       <c r="A26" s="56" t="s">
         <v>47</v>
       </c>
@@ -26041,7 +25862,7 @@
         <v>7206.8030976839436</v>
       </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:34">
       <c r="A27" s="56" t="s">
         <v>48</v>
       </c>
@@ -26162,246 +25983,246 @@
         <v>4003.9951704216178</v>
       </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:34">
       <c r="A28" s="56" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="79">
         <f>B17</f>
-        <v>1101</v>
+        <v>0</v>
       </c>
       <c r="C28" s="79">
         <f t="shared" ref="C28:AA28" si="12">C17</f>
-        <v>716</v>
+        <v>0</v>
       </c>
       <c r="D28" s="79">
         <f t="shared" si="12"/>
-        <v>1134</v>
+        <v>0</v>
       </c>
       <c r="E28" s="79">
         <f t="shared" si="12"/>
-        <v>566</v>
+        <v>0</v>
       </c>
       <c r="F28" s="79">
         <f t="shared" si="12"/>
-        <v>1059</v>
+        <v>0</v>
       </c>
       <c r="G28" s="79">
         <f t="shared" si="12"/>
-        <v>756</v>
+        <v>0</v>
       </c>
       <c r="H28" s="79">
         <f t="shared" si="12"/>
-        <v>486</v>
+        <v>0</v>
       </c>
       <c r="I28" s="79">
         <f t="shared" si="12"/>
-        <v>556</v>
+        <v>0</v>
       </c>
       <c r="J28" s="79">
         <f t="shared" si="12"/>
-        <v>720</v>
+        <v>0</v>
       </c>
       <c r="K28" s="79">
         <f t="shared" si="12"/>
-        <v>551</v>
+        <v>0</v>
       </c>
       <c r="L28" s="79">
         <f t="shared" si="12"/>
-        <v>1940.443</v>
+        <v>0</v>
       </c>
       <c r="M28" s="79">
         <f t="shared" si="12"/>
-        <v>815.92899999999997</v>
+        <v>0</v>
       </c>
       <c r="N28" s="79">
         <f t="shared" si="12"/>
-        <v>717.85</v>
+        <v>0</v>
       </c>
       <c r="O28" s="79">
         <f t="shared" si="12"/>
-        <v>791.077</v>
+        <v>0</v>
       </c>
       <c r="P28" s="79">
         <f t="shared" si="12"/>
-        <v>733.03200000000004</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="79">
         <f t="shared" si="12"/>
-        <v>532.48900000000003</v>
+        <v>0</v>
       </c>
       <c r="R28" s="79">
         <f t="shared" si="12"/>
-        <v>3970.3082495268764</v>
+        <v>0</v>
       </c>
       <c r="S28" s="79">
         <f t="shared" si="12"/>
-        <v>4192.6286449138051</v>
+        <v>0</v>
       </c>
       <c r="T28" s="79">
         <f t="shared" si="12"/>
-        <v>4414.949040300733</v>
+        <v>0</v>
       </c>
       <c r="U28" s="79">
         <f t="shared" si="12"/>
-        <v>3291.4639995021262</v>
+        <v>0</v>
       </c>
       <c r="V28" s="79">
         <f t="shared" si="12"/>
-        <v>3759.4718080810035</v>
+        <v>0</v>
       </c>
       <c r="W28" s="79">
         <f t="shared" si="12"/>
-        <v>4227.4796166598808</v>
+        <v>0</v>
       </c>
       <c r="X28" s="79">
         <f t="shared" si="12"/>
-        <v>4695.487388726503</v>
+        <v>0</v>
       </c>
       <c r="Y28" s="79">
         <f t="shared" si="12"/>
-        <v>4878.8951776095064</v>
+        <v>0</v>
       </c>
       <c r="Z28" s="79">
         <f t="shared" si="12"/>
-        <v>5062.3029664925089</v>
+        <v>0</v>
       </c>
       <c r="AA28" s="79">
         <f t="shared" si="12"/>
-        <v>5290.3481356922075</v>
+        <v>0</v>
       </c>
       <c r="AB28" s="87">
         <f t="shared" ref="AB28:AD28" si="13">AB17</f>
-        <v>5290.3481356922075</v>
+        <v>0</v>
       </c>
       <c r="AC28" s="87">
         <f t="shared" si="13"/>
-        <v>5290.3481356922075</v>
+        <v>0</v>
       </c>
       <c r="AD28" s="87">
         <f t="shared" si="13"/>
-        <v>5290.3481356922075</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29" s="56" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="79">
         <f>SUM(B25:B28)</f>
-        <v>34659</v>
+        <v>33558</v>
       </c>
       <c r="C29" s="79">
         <f t="shared" ref="C29:AA29" si="14">SUM(C25:C28)</f>
-        <v>30765</v>
+        <v>30049</v>
       </c>
       <c r="D29" s="79">
         <f t="shared" si="14"/>
-        <v>31107</v>
+        <v>29973</v>
       </c>
       <c r="E29" s="79">
         <f t="shared" si="14"/>
-        <v>27403</v>
+        <v>26837</v>
       </c>
       <c r="F29" s="79">
         <f t="shared" si="14"/>
-        <v>24108</v>
+        <v>23049</v>
       </c>
       <c r="G29" s="79">
         <f t="shared" si="14"/>
-        <v>23577</v>
+        <v>22821</v>
       </c>
       <c r="H29" s="79">
         <f t="shared" si="14"/>
-        <v>23066</v>
+        <v>22580</v>
       </c>
       <c r="I29" s="79">
         <f t="shared" si="14"/>
-        <v>22730</v>
+        <v>22174</v>
       </c>
       <c r="J29" s="79">
         <f t="shared" si="14"/>
-        <v>22570</v>
+        <v>21850</v>
       </c>
       <c r="K29" s="79">
         <f t="shared" si="14"/>
-        <v>22042</v>
+        <v>21491</v>
       </c>
       <c r="L29" s="79">
         <f t="shared" si="14"/>
-        <v>20871.235000000001</v>
+        <v>18930.792000000001</v>
       </c>
       <c r="M29" s="79">
         <f t="shared" si="14"/>
-        <v>19530.183000000001</v>
+        <v>18714.254000000001</v>
       </c>
       <c r="N29" s="79">
         <f t="shared" si="14"/>
-        <v>18781.439000000002</v>
+        <v>18063.589000000004</v>
       </c>
       <c r="O29" s="79">
         <f t="shared" si="14"/>
-        <v>18269.941999999999</v>
+        <v>17478.864999999998</v>
       </c>
       <c r="P29" s="79">
         <f t="shared" si="14"/>
-        <v>17512.342000000001</v>
+        <v>16779.310000000001</v>
       </c>
       <c r="Q29" s="79">
         <f t="shared" si="14"/>
-        <v>17111.263000000003</v>
+        <v>16578.774000000001</v>
       </c>
       <c r="R29" s="79">
         <f t="shared" si="14"/>
-        <v>20289.449086873428</v>
+        <v>16319.140837346553</v>
       </c>
       <c r="S29" s="79">
         <f t="shared" si="14"/>
-        <v>19910.9699887202</v>
+        <v>15718.341343806394</v>
       </c>
       <c r="T29" s="79">
         <f t="shared" si="14"/>
-        <v>19513.838971111796</v>
+        <v>15098.889930811063</v>
       </c>
       <c r="U29" s="79">
         <f t="shared" si="14"/>
-        <v>17753.005659169496</v>
+        <v>14461.541659667368</v>
       </c>
       <c r="V29" s="79">
         <f t="shared" si="14"/>
-        <v>17901.738045132202</v>
+        <v>14142.266237051201</v>
       </c>
       <c r="W29" s="79">
         <f t="shared" si="14"/>
-        <v>18050.470431094916</v>
+        <v>13822.990814435034</v>
       </c>
       <c r="X29" s="79">
         <f t="shared" si="14"/>
-        <v>17758.856144507652</v>
+        <v>13063.36875578115</v>
       </c>
       <c r="Y29" s="79">
         <f t="shared" si="14"/>
-        <v>17593.197218669509</v>
+        <v>12714.302041060002</v>
       </c>
       <c r="Z29" s="79">
         <f t="shared" si="14"/>
-        <v>17835.013588387945</v>
+        <v>12772.710621895436</v>
       </c>
       <c r="AA29" s="79">
         <f t="shared" si="14"/>
-        <v>18154.286815938198</v>
+        <v>12863.938680245989</v>
       </c>
       <c r="AB29" s="87">
         <f t="shared" ref="AB29:AD29" si="15">SUM(AB25:AB28)</f>
-        <v>17812.738867690328</v>
+        <v>12522.390731998119</v>
       </c>
       <c r="AC29" s="87">
         <f t="shared" si="15"/>
-        <v>17471.190919442459</v>
+        <v>12180.84278375025</v>
       </c>
       <c r="AD29" s="87">
         <f t="shared" si="15"/>
-        <v>17129.642971194589</v>
+        <v>11839.294835502382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove blank sheet1. Also change Miscellaneous sector correction to be zero instead of blank.
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/USA/national_tier1_caps.xlsx
+++ b/input/emissions-inventories/USA/national_tier1_caps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21980" windowHeight="14040" tabRatio="706" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28740" windowHeight="17140" tabRatio="706" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="VOC" sheetId="8" r:id="rId9"/>
     <sheet name="NH3" sheetId="9" r:id="rId10"/>
     <sheet name="NH3-Org_and_Adj" sheetId="13" r:id="rId11"/>
-    <sheet name="Sheet1" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -866,7 +865,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="279">
+  <cellStyleXfs count="283">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -966,6 +965,10 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1341,7 +1344,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="279">
+  <cellStyles count="283">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 2" xfId="86"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
@@ -1479,6 +1482,8 @@
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1574,6 +1579,8 @@
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2543,11 +2550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2079372456"/>
-        <c:axId val="2079375624"/>
+        <c:axId val="1814743384"/>
+        <c:axId val="1814745928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2079372456"/>
+        <c:axId val="1814743384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1970.0"/>
@@ -2558,12 +2565,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079375624"/>
+        <c:crossAx val="1814745928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2079375624"/>
+        <c:axId val="1814745928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2586,14 +2593,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079372456"/>
+        <c:crossAx val="1814743384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3107,11 +3113,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090156104"/>
-        <c:axId val="2090765304"/>
+        <c:axId val="1817679592"/>
+        <c:axId val="1817682472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090156104"/>
+        <c:axId val="1817679592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1990.0"/>
@@ -3122,12 +3128,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090765304"/>
+        <c:crossAx val="1817682472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090765304"/>
+        <c:axId val="1817682472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3157,7 +3163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090156104"/>
+        <c:crossAx val="1817679592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6090,11 +6096,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8555,7 +8561,7 @@
         <v>2903.2392709457517</v>
       </c>
       <c r="G42" s="95">
-        <f t="shared" si="14"/>
+        <f>G20*($L$37/$L$36)</f>
         <v>2944.3678819179149</v>
       </c>
       <c r="H42" s="95">
@@ -8639,23 +8645,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8778,10 +8767,10 @@
   <dimension ref="A1:AD32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AD12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="S12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
+      <selection pane="bottomRight" activeCell="S52" sqref="S52:U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10121,35 +10110,93 @@
       <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="67"/>
-      <c r="P18" s="67"/>
-      <c r="Q18" s="67"/>
-      <c r="R18" s="85"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="85"/>
-      <c r="X18" s="85"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="90"/>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
+      <c r="B18" s="90">
+        <v>0</v>
+      </c>
+      <c r="C18" s="90">
+        <v>0</v>
+      </c>
+      <c r="D18" s="90">
+        <v>0</v>
+      </c>
+      <c r="E18" s="90">
+        <v>0</v>
+      </c>
+      <c r="F18" s="90">
+        <v>0</v>
+      </c>
+      <c r="G18" s="90">
+        <v>0</v>
+      </c>
+      <c r="H18" s="90">
+        <v>0</v>
+      </c>
+      <c r="I18" s="90">
+        <v>0</v>
+      </c>
+      <c r="J18" s="90">
+        <v>0</v>
+      </c>
+      <c r="K18" s="90">
+        <v>0</v>
+      </c>
+      <c r="L18" s="90">
+        <v>0</v>
+      </c>
+      <c r="M18" s="90">
+        <v>0</v>
+      </c>
+      <c r="N18" s="90">
+        <v>0</v>
+      </c>
+      <c r="O18" s="90">
+        <v>0</v>
+      </c>
+      <c r="P18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="90">
+        <v>0</v>
+      </c>
+      <c r="R18" s="90">
+        <v>0</v>
+      </c>
+      <c r="S18" s="90">
+        <v>0</v>
+      </c>
+      <c r="T18" s="90">
+        <v>0</v>
+      </c>
+      <c r="U18" s="90">
+        <v>0</v>
+      </c>
+      <c r="V18" s="90">
+        <v>0</v>
+      </c>
+      <c r="W18" s="90">
+        <v>0</v>
+      </c>
+      <c r="X18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="90">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="8"/>
@@ -11205,11 +11252,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="H12" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P70" sqref="P70"/>
+      <selection pane="bottomRight" activeCell="R37" sqref="R37:S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14644,7 +14691,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -16033,35 +16080,93 @@
       <c r="A18" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="90"/>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
+      <c r="B18" s="90">
+        <v>0</v>
+      </c>
+      <c r="C18" s="90">
+        <v>0</v>
+      </c>
+      <c r="D18" s="90">
+        <v>0</v>
+      </c>
+      <c r="E18" s="90">
+        <v>0</v>
+      </c>
+      <c r="F18" s="90">
+        <v>0</v>
+      </c>
+      <c r="G18" s="90">
+        <v>0</v>
+      </c>
+      <c r="H18" s="90">
+        <v>0</v>
+      </c>
+      <c r="I18" s="90">
+        <v>0</v>
+      </c>
+      <c r="J18" s="90">
+        <v>0</v>
+      </c>
+      <c r="K18" s="90">
+        <v>0</v>
+      </c>
+      <c r="L18" s="90">
+        <v>0</v>
+      </c>
+      <c r="M18" s="90">
+        <v>0</v>
+      </c>
+      <c r="N18" s="90">
+        <v>0</v>
+      </c>
+      <c r="O18" s="90">
+        <v>0</v>
+      </c>
+      <c r="P18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="90">
+        <v>0</v>
+      </c>
+      <c r="R18" s="90">
+        <v>0</v>
+      </c>
+      <c r="S18" s="90">
+        <v>0</v>
+      </c>
+      <c r="T18" s="90">
+        <v>0</v>
+      </c>
+      <c r="U18" s="90">
+        <v>0</v>
+      </c>
+      <c r="V18" s="90">
+        <v>0</v>
+      </c>
+      <c r="W18" s="90">
+        <v>0</v>
+      </c>
+      <c r="X18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="90">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:30">
       <c r="B19" s="86"/>
@@ -21194,7 +21299,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18:AH18"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18:AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22534,35 +22639,93 @@
       <c r="A18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="90"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="90"/>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
+      <c r="B18" s="90">
+        <v>0</v>
+      </c>
+      <c r="C18" s="90">
+        <v>0</v>
+      </c>
+      <c r="D18" s="90">
+        <v>0</v>
+      </c>
+      <c r="E18" s="90">
+        <v>0</v>
+      </c>
+      <c r="F18" s="90">
+        <v>0</v>
+      </c>
+      <c r="G18" s="90">
+        <v>0</v>
+      </c>
+      <c r="H18" s="90">
+        <v>0</v>
+      </c>
+      <c r="I18" s="90">
+        <v>0</v>
+      </c>
+      <c r="J18" s="90">
+        <v>0</v>
+      </c>
+      <c r="K18" s="90">
+        <v>0</v>
+      </c>
+      <c r="L18" s="90">
+        <v>0</v>
+      </c>
+      <c r="M18" s="90">
+        <v>0</v>
+      </c>
+      <c r="N18" s="90">
+        <v>0</v>
+      </c>
+      <c r="O18" s="90">
+        <v>0</v>
+      </c>
+      <c r="P18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="90">
+        <v>0</v>
+      </c>
+      <c r="R18" s="90">
+        <v>0</v>
+      </c>
+      <c r="S18" s="90">
+        <v>0</v>
+      </c>
+      <c r="T18" s="90">
+        <v>0</v>
+      </c>
+      <c r="U18" s="90">
+        <v>0</v>
+      </c>
+      <c r="V18" s="90">
+        <v>0</v>
+      </c>
+      <c r="W18" s="90">
+        <v>0</v>
+      </c>
+      <c r="X18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="90">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="90">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="90">
+        <v>0</v>
+      </c>
       <c r="AE18" s="88"/>
       <c r="AF18" s="88"/>
       <c r="AG18" s="88"/>
@@ -23743,7 +23906,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17:AH17"/>
+      <selection pane="bottomRight" activeCell="AD17" sqref="B17:AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -25051,35 +25214,93 @@
       <c r="A17" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-      <c r="J17" s="90"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="90"/>
-      <c r="O17" s="90"/>
-      <c r="P17" s="90"/>
-      <c r="Q17" s="90"/>
-      <c r="R17" s="90"/>
-      <c r="S17" s="90"/>
-      <c r="T17" s="90"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="90"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="90"/>
-      <c r="Z17" s="90"/>
-      <c r="AA17" s="90"/>
-      <c r="AB17" s="90"/>
-      <c r="AC17" s="90"/>
-      <c r="AD17" s="90"/>
+      <c r="B17" s="90">
+        <v>0</v>
+      </c>
+      <c r="C17" s="90">
+        <v>0</v>
+      </c>
+      <c r="D17" s="90">
+        <v>0</v>
+      </c>
+      <c r="E17" s="90">
+        <v>0</v>
+      </c>
+      <c r="F17" s="90">
+        <v>0</v>
+      </c>
+      <c r="G17" s="90">
+        <v>0</v>
+      </c>
+      <c r="H17" s="90">
+        <v>0</v>
+      </c>
+      <c r="I17" s="90">
+        <v>0</v>
+      </c>
+      <c r="J17" s="90">
+        <v>0</v>
+      </c>
+      <c r="K17" s="90">
+        <v>0</v>
+      </c>
+      <c r="L17" s="90">
+        <v>0</v>
+      </c>
+      <c r="M17" s="90">
+        <v>0</v>
+      </c>
+      <c r="N17" s="90">
+        <v>0</v>
+      </c>
+      <c r="O17" s="90">
+        <v>0</v>
+      </c>
+      <c r="P17" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="90">
+        <v>0</v>
+      </c>
+      <c r="R17" s="90">
+        <v>0</v>
+      </c>
+      <c r="S17" s="90">
+        <v>0</v>
+      </c>
+      <c r="T17" s="90">
+        <v>0</v>
+      </c>
+      <c r="U17" s="90">
+        <v>0</v>
+      </c>
+      <c r="V17" s="90">
+        <v>0</v>
+      </c>
+      <c r="W17" s="90">
+        <v>0</v>
+      </c>
+      <c r="X17" s="90">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="90">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="90">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="90">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="90">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="90">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="90">
+        <v>0</v>
+      </c>
       <c r="AE17" s="88"/>
       <c r="AF17" s="88"/>
       <c r="AG17" s="88"/>
@@ -26227,6 +26448,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>